<commit_message>
Process map files, diagrams, user stories were uploaded.
</commit_message>
<xml_diff>
--- a/trim_1/req_func_nofunc/PL02 - Historias de Usuario.xlsx
+++ b/trim_1/req_func_nofunc/PL02 - Historias de Usuario.xlsx
@@ -3,7 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="V1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="V1" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,238 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="93">
+  <si>
+    <t>Columna 1</t>
+  </si>
+  <si>
+    <t>Historia de usuarios</t>
+  </si>
+  <si>
+    <t>Actor</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Prioridad</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>HU001</t>
+  </si>
+  <si>
+    <t>Iniciar Sesión</t>
+  </si>
+  <si>
+    <t>Cliente, Administrador</t>
+  </si>
+  <si>
+    <t>Acceder a la plataforma con credenciales válidas.</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Por definir</t>
+  </si>
+  <si>
+    <t>HU002</t>
+  </si>
+  <si>
+    <t>Navegar por Categorías</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Explorar productos organizados en categorías y subcategorías.</t>
+  </si>
+  <si>
+    <t>HU003</t>
+  </si>
+  <si>
+    <t>Recuperar Contraseña</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Restablecer contraseña olvidada.</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>HU004</t>
+  </si>
+  <si>
+    <t>Cerrar Sesión</t>
+  </si>
+  <si>
+    <t>Terminar la sesión de forma segura.</t>
+  </si>
+  <si>
+    <t>Baja</t>
+  </si>
+  <si>
+    <t>HU005</t>
+  </si>
+  <si>
+    <t>Búsqueda Avanzada</t>
+  </si>
+  <si>
+    <t>Realizar búsquedas detalladas utilizando filtros y operadores.</t>
+  </si>
+  <si>
+    <t>HU006</t>
+  </si>
+  <si>
+    <t>Registro de Usuario</t>
+  </si>
+  <si>
+    <t>Nuevo Usuario</t>
+  </si>
+  <si>
+    <t>Crear una nueva cuenta.</t>
+  </si>
+  <si>
+    <t>HU007</t>
+  </si>
+  <si>
+    <t>Perfil de Usuario</t>
+  </si>
+  <si>
+    <t>Usuario Registrado</t>
+  </si>
+  <si>
+    <t>Ver y editar información personal.</t>
+  </si>
+  <si>
+    <t>HU008</t>
+  </si>
+  <si>
+    <t>Historial de Pedidos</t>
+  </si>
+  <si>
+    <t>Ver y gestionar pedidos anteriores.</t>
+  </si>
+  <si>
+    <t>HU009</t>
+  </si>
+  <si>
+    <t>Lista de Deseos</t>
+  </si>
+  <si>
+    <t>Guardar productos para futuras compras.</t>
+  </si>
+  <si>
+    <t>HU010</t>
+  </si>
+  <si>
+    <t>Agregar/Eliminar Productos del Carrito</t>
+  </si>
+  <si>
+    <t>Modificar el contenido del carrito de compras.</t>
+  </si>
+  <si>
+    <t>HU011</t>
+  </si>
+  <si>
+    <t>Aplicar Cupones</t>
+  </si>
+  <si>
+    <t>Utilizar códigos de descuento.</t>
+  </si>
+  <si>
+    <t>HU012</t>
+  </si>
+  <si>
+    <t>Calcular Costo Total</t>
+  </si>
+  <si>
+    <t>Ver el precio final de la compra.</t>
+  </si>
+  <si>
+    <t>HU013</t>
+  </si>
+  <si>
+    <t>Seleccionar Envío y Pago</t>
+  </si>
+  <si>
+    <t>Elegir opciones de envío y pago.</t>
+  </si>
+  <si>
+    <t>HU014</t>
+  </si>
+  <si>
+    <t>Confirmación de Pedido</t>
+  </si>
+  <si>
+    <t>Recibir un correo de confirmación.</t>
+  </si>
+  <si>
+    <t>HU015</t>
+  </si>
+  <si>
+    <t>Contactar Servicio al Cliente</t>
+  </si>
+  <si>
+    <t>Obtener asistencia para consultas o problemas.</t>
+  </si>
+  <si>
+    <t>HU016</t>
+  </si>
+  <si>
+    <t>Recomendaciones de Productos</t>
+  </si>
+  <si>
+    <t>Recibir sugerencias personalizadas.</t>
+  </si>
+  <si>
+    <t>HU017</t>
+  </si>
+  <si>
+    <t>Calificar y Resenñar Productos</t>
+  </si>
+  <si>
+    <t>Evaluar productos y compartir opiniones.</t>
+  </si>
+  <si>
+    <t>HU018</t>
+  </si>
+  <si>
+    <t>Moderar Valoraciones</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>Revisar y aprobar reseñas.</t>
+  </si>
+  <si>
+    <t>HU019</t>
+  </si>
+  <si>
+    <t>Configurar Métodos de Pago</t>
+  </si>
+  <si>
+    <t>Agregar y gestionar opciones de pago.</t>
+  </si>
+  <si>
+    <t>HU020</t>
+  </si>
+  <si>
+    <t>Procesar Pagos</t>
+  </si>
+  <si>
+    <t>Sistema</t>
+  </si>
+  <si>
+    <t>Gestionar transacciones de pago.</t>
+  </si>
   <si>
     <t xml:space="preserve">Código </t>
   </si>
@@ -22,24 +254,15 @@
     <t xml:space="preserve">Fecha </t>
   </si>
   <si>
-    <t>HU001</t>
-  </si>
-  <si>
     <t>Iniciar sesion</t>
   </si>
   <si>
-    <t>Descripción</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Describe la necesidad de diferentes roles (cliente, administrador, ayudante) de iniciar sesión para acceder a funcionalidades de la plataforma.</t>
   </si>
   <si>
     <t>Estimación</t>
   </si>
   <si>
-    <t>Prioridad</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dependencia </t>
   </si>
   <si>
@@ -62,9 +285,6 @@
   </si>
   <si>
     <t>Fecha</t>
-  </si>
-  <si>
-    <t>HU002</t>
   </si>
   <si>
     <t>Categorias</t>
@@ -77,10 +297,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -121,8 +346,176 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="17">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF284E3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF356854"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF284E3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF356854"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF356854"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF284E3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF356854"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF284E3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF284E3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF284E3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF284E3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -171,43 +564,142 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="13" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="15" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="16" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="13" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF356854"/>
+          <bgColor rgb="FF356854"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8F9FA"/>
+          <bgColor rgb="FFF8F9FA"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1">
+    <tableStyle count="3" pivot="0" name="Hoja 1-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+  </tableStyles>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:F21" displayName="Tabla_1" name="Tabla_1" id="1">
+  <tableColumns count="6">
+    <tableColumn name="Columna 1" id="1"/>
+    <tableColumn name="Historia de usuarios" id="2"/>
+    <tableColumn name="Actor" id="3"/>
+    <tableColumn name="Descripción" id="4"/>
+    <tableColumn name="Prioridad" id="5"/>
+    <tableColumn name="Estado" id="6"/>
+  </tableColumns>
+  <tableStyleInfo name="Hoja 1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,6 +902,454 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="13.5"/>
+    <col customWidth="1" min="2" max="2" width="30.88"/>
+    <col customWidth="1" min="3" max="3" width="25.25"/>
+    <col customWidth="1" min="4" max="4" width="37.63"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
@@ -425,237 +1365,331 @@
     <row r="2" ht="15.75" customHeight="1"/>
     <row r="3" ht="15.75" customHeight="1"/>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
+      <c r="B4" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="15"/>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="B6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+    </row>
+    <row r="7" ht="81.0" customHeight="1">
+      <c r="B7" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="B8" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" ht="81.0" customHeight="1">
-      <c r="B7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
+      <c r="D8" s="13" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="B9" s="8">
+      <c r="B9" s="20">
         <v>5.0</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="20">
         <v>5.0</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="15"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="D10" s="18"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="B11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>13</v>
+      <c r="B11" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="B16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>16</v>
+      <c r="B16" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
     </row>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="B19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>2</v>
+      <c r="B19" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="B20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="3"/>
+      <c r="B20" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="15"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="B21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
+      <c r="B21" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="18"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="B22" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
+      <c r="B22" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="B23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>9</v>
+      <c r="B23" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="B24" s="8">
+      <c r="B24" s="20">
         <v>5.0</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="20">
         <v>5.0</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="15"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="B25" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
+      <c r="B25" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="B26" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>13</v>
+      <c r="B26" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="B31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="1" t="s">
+      <c r="B31" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1"/>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="B34" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="B35" s="14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
+      <c r="C35" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="15"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="B36" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="17"/>
+      <c r="D36" s="18"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="B37" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="17"/>
+      <c r="D37" s="18"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="B38" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="B39" s="20">
+        <v>5.0</v>
+      </c>
+      <c r="C39" s="20">
+        <v>5.0</v>
+      </c>
+      <c r="D39" s="15"/>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="B40" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="17"/>
+      <c r="D40" s="18"/>
+    </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="B41" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+    </row>
+    <row r="46" ht="15.75" customHeight="1">
+      <c r="B46" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" ht="15.75" customHeight="1">
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+    </row>
     <row r="48" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
@@ -1610,19 +2644,25 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B40:D40"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B36:D36"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B9:C9 B24:C24">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B9:C9 B24:C24 B39:C39">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
   </dataValidations>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>